<commit_message>
hola equipo, ¿que mas? ¿que me cuentan?
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Desktop\UANDES\SEMESTRE6\REDES\ServidorTCPInfracom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orjue\Desktop\INFRACOM\parcial2\ServidorTCPInfracom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2D48B2-CC2F-4D41-B1B4-5EA779F5D511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70098C42-D6AA-40FD-80E2-739BB6F2D265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFA708B9-7D67-4C96-9293-ED598A1B6F45}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AFA708B9-7D67-4C96-9293-ED598A1B6F45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -193,8 +193,2234 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Tasa cliente vs Número conexiones (100MB)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.0735884576192442E-3"/>
+                  <c:y val="-0.47457385535141439"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>129774.25742574257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52318.930246482385</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30251.456926894007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1D3-47BC-AE75-4665043605F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="244852336"/>
+        <c:axId val="244852752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="244852336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Número conexiones</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244852752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="244852752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Tasa</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CO" baseline="0"/>
+                  <a:t> cliente (B/ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="244852336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1400" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Tasa cliente vs Número conexiones (250MB)</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.12208122283095385"/>
+                  <c:y val="-0.44000619714202394"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$7:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>128944.41711756025</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58501.227404597186</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29736.376423612684</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-35CA-4DD8-B97C-2072ACB0EEC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="16503792"/>
+        <c:axId val="16504624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="16503792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Número conexiones</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16504624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="16504624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO" sz="900" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Tasa cliente (B/ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CO" sz="900">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16503792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>73819</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E96417D-AB11-4D7F-9E75-25EBF75A5CFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>550068</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>102393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>178593</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B76DBA6F-676C-4112-A1EB-EDB821640AD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -492,29 +2718,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B8AE9D-C93C-471E-AD75-FC13434A0BE5}">
   <dimension ref="A2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -546,7 +2772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -579,7 +2805,7 @@
         <v>25505</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -614,7 +2840,7 @@
         <v>25505</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -649,7 +2875,7 @@
         <v>25505</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -682,7 +2908,7 @@
         <v>25505</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -717,7 +2943,7 @@
         <v>25505</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -752,7 +2978,7 @@
         <v>25505</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -760,7 +2986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
@@ -780,7 +3006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0</v>
       </c>
@@ -800,7 +3026,7 @@
         <v>3115</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>1</v>
       </c>
@@ -820,7 +3046,7 @@
         <v>3645</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>2</v>
       </c>
@@ -840,7 +3066,7 @@
         <v>3497</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>3</v>
       </c>
@@ -860,7 +3086,7 @@
         <v>2647</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>4</v>
       </c>
@@ -880,7 +3106,7 @@
         <v>3595</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -888,7 +3114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
@@ -908,7 +3134,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>0</v>
       </c>
@@ -928,7 +3154,7 @@
         <v>7604</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>1</v>
       </c>
@@ -948,7 +3174,7 @@
         <v>7963</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -968,7 +3194,7 @@
         <v>7909</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>3</v>
       </c>
@@ -988,7 +3214,7 @@
         <v>7155</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>4</v>
       </c>
@@ -1008,7 +3234,7 @@
         <v>7040</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>5</v>
       </c>
@@ -1028,7 +3254,7 @@
         <v>6493</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>6</v>
       </c>
@@ -1048,7 +3274,7 @@
         <v>7011</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>7</v>
       </c>
@@ -1068,7 +3294,7 @@
         <v>7406</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>8</v>
       </c>
@@ -1088,7 +3314,7 @@
         <v>7341</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>9</v>
       </c>
@@ -1111,5 +3337,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>